<commit_message>
Elimino max(dmax()) en distr normal
</commit_message>
<xml_diff>
--- a/posts/clima-economist/distr-normal.xlsx
+++ b/posts/clima-economist/distr-normal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/34bf2af71bbc2e43/Documentos/GitHub/industrial-stats/hojas-excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/34bf2af71bbc2e43/Documentos/GitHub/blog/posts/clima-economist/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="319" documentId="8_{56F7861F-2369-4636-8BD1-46CD89C110AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAB6ECDA-9F8A-495F-96C5-0D073BB885AA}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31245" yWindow="2775" windowWidth="14055" windowHeight="11985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inicio" sheetId="4" r:id="rId1"/>
@@ -181,7 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -200,8 +200,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -10502,10 +10500,6 @@
 </c:userShapes>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -10808,7 +10802,7 @@
   </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -10821,43 +10815,40 @@
       <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="18" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="18" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="18" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="19"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2">
         <v>250</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15">
+      <c r="C2" s="3"/>
+      <c r="D2">
         <v>253</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15">
+      <c r="F2">
         <v>250</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15">
+      <c r="H2">
         <v>253</v>
       </c>
-      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -10866,7 +10857,7 @@
       <c r="B3" s="10">
         <v>7</v>
       </c>
-      <c r="C3" s="16"/>
+      <c r="C3" s="14"/>
       <c r="D3" s="10">
         <v>7</v>
       </c>
@@ -12198,7 +12189,7 @@
   </sheetPr>
   <dimension ref="A2:I40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>

</xml_diff>